<commit_message>
Seems to be the final file
</commit_message>
<xml_diff>
--- a/risk_value_final_version.xlsx
+++ b/risk_value_final_version.xlsx
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericagoto/Dropbox/ESTUDOS/erica phD/methodology/AHP/BGM-Weight02-MultilinerLogistic/BGM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85493FF6-18DA-5E4A-9193-C70D4D133507}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E044124-85E5-D640-9369-D1A96AEBF26F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30820" yWindow="2480" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="1360" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -4520,16 +4531,16 @@
   <dimension ref="A1:X740"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:L1048576"/>
+      <selection activeCell="B1" sqref="B1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="12" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="14" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="16.83203125" style="3" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="10.83203125" customWidth="1"/>
+    <col min="8" max="12" width="10.83203125" customWidth="1"/>
+    <col min="14" max="16" width="10.83203125" customWidth="1"/>
+    <col min="17" max="17" width="16.83203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" customWidth="1"/>
     <col min="19" max="19" width="10.83203125" style="2"/>
   </cols>
   <sheetData>

</xml_diff>